<commit_message>
Improve blank cell handling and example
</commit_message>
<xml_diff>
--- a/Assets/Example/Excels/MstItems.xlsx
+++ b/Assets/Example/Excels/MstItems.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="4780" yWindow="40" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -87,18 +87,34 @@
     <t>Blue</t>
   </si>
   <si>
-    <t># This row is comment.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Red</t>
+  </si>
+  <si>
+    <t># This row is a comment.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>no entry item</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Red</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The first cell in the blank means the end of the row.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The blank header cell means the end of the column</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +125,24 @@
     </font>
     <font>
       <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
@@ -162,10 +196,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -177,9 +213,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -508,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -519,9 +563,10 @@
     <col min="1" max="1" width="7.1640625" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="45.83203125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1">
+    <row r="1" spans="1:8" s="5" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -540,8 +585,11 @@
       <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="H1" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -558,10 +606,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -581,7 +629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -601,7 +649,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -621,7 +669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -641,7 +689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -661,9 +709,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -671,7 +719,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -691,7 +739,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -711,7 +759,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -731,7 +779,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -751,17 +799,40 @@
         <v>18</v>
       </c>
     </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4">
+        <v>99</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F12">
-      <formula1>"Red,Green,Blue"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12">
       <formula1>"Red,Green,Blue"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Implementation of formula cell import feature
</commit_message>
<xml_diff>
--- a/Assets/Example/Excels/MstItems.xlsx
+++ b/Assets/Example/Excels/MstItems.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -107,6 +107,14 @@
   </si>
   <si>
     <t>The blank header cell means the end of the column</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>hiddenCoefficient</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Base Factor ( Column 'E' = 'H3' * Column 'I' )</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -149,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +194,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -196,12 +216,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -219,11 +249,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -552,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -564,9 +614,10 @@
     <col min="3" max="3" width="8.1640625" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="45.83203125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1">
+    <row r="1" spans="1:9" s="5" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -588,8 +639,11 @@
       <c r="H1" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -603,13 +657,20 @@
         <v>0</v>
       </c>
       <c r="E2" s="3">
-        <v>1.1000000000000001</v>
+        <f>$H$3*I2</f>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -623,13 +684,20 @@
         <v>0</v>
       </c>
       <c r="E3" s="3">
-        <v>1.4</v>
+        <f t="shared" ref="E3:E12" si="0">$H$3*I3</f>
+        <v>3.2199999999999998</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="H3" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -643,13 +711,17 @@
         <v>0</v>
       </c>
       <c r="E4" s="3">
-        <v>1.6</v>
+        <f t="shared" si="0"/>
+        <v>3.6799999999999997</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="2">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -663,13 +735,17 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>1.8</v>
+        <f t="shared" si="0"/>
+        <v>4.1399999999999997</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="2">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -683,13 +759,17 @@
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>2.1</v>
+        <f t="shared" si="0"/>
+        <v>4.83</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="2">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -703,13 +783,17 @@
         <v>0</v>
       </c>
       <c r="E7" s="2">
-        <v>2.2000000000000002</v>
+        <f t="shared" si="0"/>
+        <v>5.0599999999999996</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
@@ -718,8 +802,9 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -733,13 +818,17 @@
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>2.4</v>
+        <f t="shared" si="0"/>
+        <v>5.52</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="2">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -753,13 +842,17 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>2.6</v>
+        <f t="shared" si="0"/>
+        <v>5.9799999999999995</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="2">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -773,13 +866,17 @@
         <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>2.8</v>
+        <f t="shared" si="0"/>
+        <v>6.4399999999999995</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="2">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -793,18 +890,22 @@
         <v>1</v>
       </c>
       <c r="E12" s="1">
-        <v>3.5</v>
+        <f t="shared" si="0"/>
+        <v>8.0499999999999989</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I12" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="4">
         <v>99</v>
       </c>
@@ -818,10 +919,14 @@
         <v>0</v>
       </c>
       <c r="E15" s="4">
-        <v>1</v>
+        <f t="shared" ref="E15" si="1">$H$3*I15</f>
+        <v>22.77</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>22</v>
+      </c>
+      <c r="I15" s="2">
+        <v>9.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>